<commit_message>
Update to hist summary.
</commit_message>
<xml_diff>
--- a/07_calc_country_stats/03_total_c_stats/02_combine_tile_stats/country_total_c_hists_summary.xlsx
+++ b/07_calc_country_stats/03_total_c_stats/02_combine_tile_stats/country_total_c_hists_summary.xlsx
@@ -22,22 +22,22 @@
     <t>Country_Code</t>
   </si>
   <si>
-    <t>0-700</t>
-  </si>
-  <si>
-    <t>700-1400</t>
-  </si>
-  <si>
-    <t>1400-2100</t>
-  </si>
-  <si>
-    <t>2100-2800</t>
-  </si>
-  <si>
-    <t>2800-3500</t>
-  </si>
-  <si>
-    <t>3500-</t>
+    <t>0-250</t>
+  </si>
+  <si>
+    <t>250-500</t>
+  </si>
+  <si>
+    <t>500-750</t>
+  </si>
+  <si>
+    <t>750-1000</t>
+  </si>
+  <si>
+    <t>1000-1250</t>
+  </si>
+  <si>
+    <t>1250-</t>
   </si>
   <si>
     <t>Angola</t>
@@ -1170,13 +1170,13 @@
         <v>130</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.692303047583905</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.3076030257795072</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>9.392663658777947E-05</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1199,10 +1199,10 @@
         <v>131</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1286,22 +1286,22 @@
         <v>134</v>
       </c>
       <c r="D6">
-        <v>0.9906225740092743</v>
+        <v>0.1609043747883557</v>
       </c>
       <c r="E6">
-        <v>0.009244968336861697</v>
+        <v>0.6651602967972892</v>
       </c>
       <c r="F6">
-        <v>0.0001002070946623021</v>
+        <v>0.1698181989905575</v>
       </c>
       <c r="G6">
-        <v>1.84288909723774E-05</v>
+        <v>0.003635098744301441</v>
       </c>
       <c r="H6">
-        <v>6.910834114641523E-06</v>
+        <v>0.0002885273242862836</v>
       </c>
       <c r="I6">
-        <v>6.910834114641523E-06</v>
+        <v>0.0001935033552099627</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1315,10 +1315,10 @@
         <v>135</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.9606119791666666</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.03938802083333334</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1344,13 +1344,13 @@
         <v>136</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0.5942693686857415</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.4056822746953533</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>4.835661890520615E-05</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1373,19 +1373,19 @@
         <v>137</v>
       </c>
       <c r="D9">
-        <v>0.9012508571974202</v>
+        <v>0.04511766390916745</v>
       </c>
       <c r="E9">
-        <v>0.09874914280257983</v>
+        <v>0.4704212637043081</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.4201300335934584</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.06217480751035147</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.00215623128271456</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1402,16 +1402,16 @@
         <v>138</v>
       </c>
       <c r="D10">
-        <v>0.9793119919619842</v>
+        <v>0.001655370069920855</v>
       </c>
       <c r="E10">
-        <v>0.02068800803801586</v>
+        <v>0.4342093343106331</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.5557184388460177</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.008416856773428428</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1431,13 +1431,13 @@
         <v>139</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0.6536685279938942</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.3463288760127619</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>2.595993343873066E-06</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1489,10 +1489,10 @@
         <v>141</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0.7521936372265473</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.2478063627734526</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1518,22 +1518,22 @@
         <v>142</v>
       </c>
       <c r="D14">
-        <v>0.8893973247790306</v>
+        <v>0.05865930173216054</v>
       </c>
       <c r="E14">
-        <v>0.1106026752209695</v>
+        <v>0.5028411893111242</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.3608760726829833</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.07013127366764303</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>0.007436410966776312</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>5.575163931262517E-05</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1547,16 +1547,16 @@
         <v>143</v>
       </c>
       <c r="D15">
-        <v>0.9946713718570799</v>
+        <v>0.05348037053374504</v>
       </c>
       <c r="E15">
-        <v>0.005328628142920159</v>
+        <v>0.8045169827966475</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.1406263784737539</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>0.001376268195853551</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1576,19 +1576,19 @@
         <v>144</v>
       </c>
       <c r="D16">
-        <v>0.9897187304073353</v>
+        <v>0.001043020387181083</v>
       </c>
       <c r="E16">
-        <v>0.01028126959266475</v>
+        <v>0.6738963849806986</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.3208918761155057</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>0.004154305521858507</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1.441299475607207E-05</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1605,10 +1605,10 @@
         <v>145</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0.7625057283468489</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.2374942716531511</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1634,13 +1634,13 @@
         <v>146</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0.312629692510847</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>0.6869458592718355</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>0.0004244482173174873</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1663,16 +1663,16 @@
         <v>147</v>
       </c>
       <c r="D19">
-        <v>0.999238443655762</v>
+        <v>0.1998097931044535</v>
       </c>
       <c r="E19">
-        <v>0.0007615563442380428</v>
+        <v>0.7733761359578484</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.02660127241854262</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>0.0002127985191555105</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1692,19 +1692,19 @@
         <v>148</v>
       </c>
       <c r="D20">
-        <v>0.9877684153302528</v>
+        <v>0.04077194889915738</v>
       </c>
       <c r="E20">
-        <v>0.01223158466974721</v>
+        <v>0.7170426746398478</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>0.2359336776297907</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>0.006115792334873607</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>0.0001359064963305246</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1721,16 +1721,16 @@
         <v>149</v>
       </c>
       <c r="D21">
-        <v>0.9991688963479697</v>
+        <v>0.02687592605501013</v>
       </c>
       <c r="E21">
-        <v>0.0008311036520303058</v>
+        <v>0.8766266843253852</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>0.09624359022479119</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>0.0002537993948135557</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1750,16 +1750,16 @@
         <v>150</v>
       </c>
       <c r="D22">
-        <v>0.9996893445169307</v>
+        <v>0.3343847826606448</v>
       </c>
       <c r="E22">
-        <v>0.0003106554830692762</v>
+        <v>0.660650703754152</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.0048928238583411</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>7.168972686214065E-05</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1779,22 +1779,22 @@
         <v>151</v>
       </c>
       <c r="D23">
-        <v>0.9846547099985671</v>
+        <v>0.05931995521073219</v>
       </c>
       <c r="E23">
-        <v>0.01534529000143292</v>
+        <v>0.7821962366606824</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.1498043448671759</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>0.00855553109487768</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>0.0001235077413039434</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>4.244252278486025E-07</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1808,22 +1808,22 @@
         <v>152</v>
       </c>
       <c r="D24">
-        <v>0.9787533128558893</v>
+        <v>0.1519414741438795</v>
       </c>
       <c r="E24">
-        <v>0.02124534816564413</v>
+        <v>0.6021216560128614</v>
       </c>
       <c r="F24">
-        <v>8.926523110322007E-07</v>
+        <v>0.2363959787798693</v>
       </c>
       <c r="G24">
-        <v>2.231630777580502E-07</v>
+        <v>0.008917150261056168</v>
       </c>
       <c r="H24">
-        <v>2.231630777580502E-07</v>
+        <v>0.0006114668330570574</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1.227396927669276E-05</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1837,13 +1837,13 @@
         <v>153</v>
       </c>
       <c r="D25">
-        <v>0.9999536998453575</v>
+        <v>0.4289801927938439</v>
       </c>
       <c r="E25">
-        <v>4.630015464251651E-05</v>
+        <v>0.5516107823800132</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.01940902482614292</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1866,19 +1866,19 @@
         <v>154</v>
       </c>
       <c r="D26">
-        <v>0.8169665377501261</v>
+        <v>0.004624180258954095</v>
       </c>
       <c r="E26">
-        <v>0.1830334622498739</v>
+        <v>0.278880107617286</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.6114007062384396</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>0.1013956616781571</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>0.003699344207163275</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1895,10 +1895,10 @@
         <v>155</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0.7564815592119991</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>0.2435184407880009</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1924,19 +1924,19 @@
         <v>156</v>
       </c>
       <c r="D28">
-        <v>0.976351016906273</v>
+        <v>0.1425648697106024</v>
       </c>
       <c r="E28">
-        <v>0.02364898309372697</v>
+        <v>0.5474574593292488</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>0.2995721183989088</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>0.01038355350719919</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>2.199905404067625E-05</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1953,16 +1953,16 @@
         <v>157</v>
       </c>
       <c r="D29">
-        <v>0.9897201599086236</v>
+        <v>0.3586521987435751</v>
       </c>
       <c r="E29">
-        <v>0.01027984009137636</v>
+        <v>0.555682467161622</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>0.0799543118218161</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>0.005711022272986865</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -1982,13 +1982,13 @@
         <v>158</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0.9933446074954995</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>0.006628116305711636</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>2.727619878893677E-05</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -2011,22 +2011,22 @@
         <v>159</v>
       </c>
       <c r="D31">
-        <v>0.9348327521665776</v>
+        <v>0.04226970783357725</v>
       </c>
       <c r="E31">
-        <v>0.0651632902211703</v>
+        <v>0.6431567291883368</v>
       </c>
       <c r="F31">
-        <v>3.957612252079252E-06</v>
+        <v>0.2707371569029791</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>0.03872988177923923</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>0.004996571503299014</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>0.0001099527925686366</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2040,19 +2040,19 @@
         <v>160</v>
       </c>
       <c r="D32">
-        <v>0.956793336803748</v>
+        <v>0.01902418248071554</v>
       </c>
       <c r="E32">
-        <v>0.04320666319625195</v>
+        <v>0.668543845534996</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>0.2855520325587999</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>0.02531825280393734</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>0.001561686621551275</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2069,10 +2069,10 @@
         <v>161</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0.8013214855320119</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>0.1986785144679881</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -2098,22 +2098,22 @@
         <v>162</v>
       </c>
       <c r="D34">
-        <v>0.9533507158933711</v>
+        <v>0.009702070991815383</v>
       </c>
       <c r="E34">
-        <v>0.0466492841066289</v>
+        <v>0.5012841189526751</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>0.467787924551691</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>0.02111352169736041</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>0.0001121825745121553</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>1.812319459000894E-07</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2127,10 +2127,10 @@
         <v>163</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0.7630676361640829</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>0.2369323638359171</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2156,19 +2156,19 @@
         <v>164</v>
       </c>
       <c r="D36">
-        <v>0.9852243994854013</v>
+        <v>0.0007979009206870022</v>
       </c>
       <c r="E36">
-        <v>0.01477560051459873</v>
+        <v>0.6659507058254548</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>0.3276716121263349</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>0.005549786547972327</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>2.999457955098114E-05</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -2185,19 +2185,19 @@
         <v>165</v>
       </c>
       <c r="D37">
-        <v>0.9936030926486038</v>
+        <v>0.3224250672030448</v>
       </c>
       <c r="E37">
-        <v>0.006396907351396215</v>
+        <v>0.5885117376333312</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>0.08589278170133061</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>0.003105609413535821</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>6.48040487575693E-05</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -2214,10 +2214,10 @@
         <v>166</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2243,19 +2243,19 @@
         <v>167</v>
       </c>
       <c r="D39">
-        <v>0.959120828226312</v>
+        <v>0.005951824025299638</v>
       </c>
       <c r="E39">
-        <v>0.040879171773688</v>
+        <v>0.6237848408012799</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>0.3555960478672143</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>0.01466494821246456</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>2.339093741520785E-06</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -2272,10 +2272,10 @@
         <v>168</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0.1363967906637491</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>0.8636032093362509</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2330,10 +2330,10 @@
         <v>170</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>0.9919864559819414</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>0.008013544018058691</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2359,10 +2359,10 @@
         <v>171</v>
       </c>
       <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
         <v>1</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -2388,16 +2388,16 @@
         <v>172</v>
       </c>
       <c r="D44">
-        <v>0.9856274184632393</v>
+        <v>0.1509121061359867</v>
       </c>
       <c r="E44">
-        <v>0.01437258153676064</v>
+        <v>0.3980099502487562</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>0.006633499170812604</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -2417,22 +2417,22 @@
         <v>173</v>
       </c>
       <c r="D45">
-        <v>0.9999948611834352</v>
+        <v>0.5182984693178392</v>
       </c>
       <c r="E45">
-        <v>4.282347137336585E-06</v>
+        <v>0.4783510222819086</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>0.00334879546139721</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>8.564694274673171E-07</v>
       </c>
       <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
         <v>8.564694274673171E-07</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2446,22 +2446,22 @@
         <v>174</v>
       </c>
       <c r="D46">
-        <v>0.9697785146120408</v>
+        <v>0.03029140034831038</v>
       </c>
       <c r="E46">
-        <v>0.03022074161178528</v>
+        <v>0.5644550854022398</v>
       </c>
       <c r="F46">
-        <v>3.718880869742107E-07</v>
+        <v>0.3937595691453379</v>
       </c>
       <c r="G46">
-        <v>3.718880869742107E-07</v>
+        <v>0.01147906958063296</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>1.375985921804579E-05</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>1.115664260922632E-06</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2475,13 +2475,13 @@
         <v>175</v>
       </c>
       <c r="D47">
-        <v>0.9795918367346939</v>
+        <v>0.01457725947521866</v>
       </c>
       <c r="E47">
-        <v>0.02040816326530612</v>
+        <v>0.5918367346938775</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>0.3935860058309038</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -2504,22 +2504,22 @@
         <v>176</v>
       </c>
       <c r="D48">
-        <v>0.9521990842796961</v>
+        <v>0.05000203990582215</v>
       </c>
       <c r="E48">
-        <v>0.04780091572030391</v>
+        <v>0.5567097108729613</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>0.3676206406883564</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>0.02464370741696596</v>
       </c>
       <c r="H48">
-        <v>0</v>
+        <v>0.001015346672123963</v>
       </c>
       <c r="I48">
-        <v>0</v>
+        <v>8.55444377032503E-06</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2533,10 +2533,10 @@
         <v>177</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0.9998730481147645</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>0.0001269518852354958</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -2562,10 +2562,10 @@
         <v>178</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0.770042194092827</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>0.229957805907173</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -2591,19 +2591,19 @@
         <v>179</v>
       </c>
       <c r="D51">
-        <v>0.989954363454132</v>
+        <v>0.06842429268441591</v>
       </c>
       <c r="E51">
-        <v>0.01004563654586803</v>
+        <v>0.6997222123294989</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>0.2276841360854324</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>0.004161727371243379</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>7.631529409370501E-06</v>
       </c>
       <c r="I51">
         <v>0</v>
@@ -2620,22 +2620,22 @@
         <v>180</v>
       </c>
       <c r="D52">
-        <v>0.9598977488100142</v>
+        <v>0.0836751214993155</v>
       </c>
       <c r="E52">
-        <v>0.04009898389702096</v>
+        <v>0.5665204511176529</v>
       </c>
       <c r="F52">
-        <v>3.015962736775066E-06</v>
+        <v>0.3268511916445768</v>
       </c>
       <c r="G52">
-        <v>2.513302280645889E-07</v>
+        <v>0.02246062849144811</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>0.0004885859633575608</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>4.021283649033422E-06</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2649,10 +2649,10 @@
         <v>181</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>0.7474120082815735</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>0.2525879917184265</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -2678,16 +2678,16 @@
         <v>182</v>
       </c>
       <c r="D54">
-        <v>0.9942857142857143</v>
+        <v>0.01142857142857143</v>
       </c>
       <c r="E54">
+        <v>0.96</v>
+      </c>
+      <c r="F54">
+        <v>0.02285714285714286</v>
+      </c>
+      <c r="G54">
         <v>0.005714285714285714</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -2707,10 +2707,10 @@
         <v>183</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>0.7662100456621005</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>0.2337899543378995</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -2736,22 +2736,22 @@
         <v>184</v>
       </c>
       <c r="D56">
-        <v>0.9928243288951755</v>
+        <v>0.015426339903447</v>
       </c>
       <c r="E56">
-        <v>0.007175671104824575</v>
+        <v>0.8184502321576828</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>0.1623547861381876</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>0.003577995756588051</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>0.0001888010823775407</v>
       </c>
       <c r="I56">
-        <v>0</v>
+        <v>1.844961717044371E-06</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2765,16 +2765,16 @@
         <v>185</v>
       </c>
       <c r="D57">
-        <v>0.9960300877559549</v>
+        <v>0.5460718763058922</v>
       </c>
       <c r="E57">
-        <v>0.003969912244045131</v>
+        <v>0.3118470539072294</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>0.1416631842875052</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>0.0004178854993731718</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -2794,22 +2794,22 @@
         <v>186</v>
       </c>
       <c r="D58">
-        <v>0.9999997282328805</v>
+        <v>0.8756624663246568</v>
       </c>
       <c r="E58">
-        <v>2.717671194941001E-07</v>
+        <v>0.1243356313055067</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>1.6306027169646E-06</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>9.058903983136669E-08</v>
       </c>
       <c r="H58">
         <v>0</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>1.811780796627334E-07</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2823,13 +2823,13 @@
         <v>187</v>
       </c>
       <c r="D59">
-        <v>0.9999670108534292</v>
+        <v>0.03087784119024841</v>
       </c>
       <c r="E59">
-        <v>3.298914657077821E-05</v>
+        <v>0.9114241414574605</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>0.0576980173522911</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2852,10 +2852,10 @@
         <v>188</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0.9636363636363636</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>0.03636363636363636</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -2881,19 +2881,19 @@
         <v>189</v>
       </c>
       <c r="D61">
-        <v>0.9815418425061382</v>
+        <v>0.006868032791879111</v>
       </c>
       <c r="E61">
-        <v>0.01845815749386179</v>
+        <v>0.6971238024523747</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>0.2887144420701107</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>0.007291560825602555</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>2.161860032927094E-06</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -2910,10 +2910,10 @@
         <v>190</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>0.9974500637484063</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>0.00254993625159371</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -2939,10 +2939,10 @@
         <v>191</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>0.01188942187956817</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <v>0.9881105781204318</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -2968,16 +2968,16 @@
         <v>192</v>
       </c>
       <c r="D64">
-        <v>0.9999989101150046</v>
+        <v>0.565500453392158</v>
       </c>
       <c r="E64">
+        <v>0.3672204009032967</v>
+      </c>
+      <c r="F64">
+        <v>0.06727805581954992</v>
+      </c>
+      <c r="G64">
         <v>1.089884995335292E-06</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-      <c r="G64">
-        <v>0</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -2997,13 +2997,13 @@
         <v>193</v>
       </c>
       <c r="D65">
-        <v>0.9997556453883379</v>
+        <v>0.3705000239042555</v>
       </c>
       <c r="E65">
-        <v>0.0002443546116620894</v>
+        <v>0.5876515928202241</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>0.04184838327552045</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -3026,10 +3026,10 @@
         <v>194</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0.9474007962085308</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>0.05259920379146919</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -3055,13 +3055,13 @@
         <v>195</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>0.9341085271317829</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>0.06589147286821706</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3084,16 +3084,16 @@
         <v>196</v>
       </c>
       <c r="D68">
-        <v>0.9983993622253454</v>
+        <v>0.3788044602554174</v>
       </c>
       <c r="E68">
-        <v>0.001600637774654609</v>
+        <v>0.5975515095471896</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>0.02321821871232292</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>0.0004258114850700572</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -3113,10 +3113,10 @@
         <v>197</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0.3247863247863248</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>0.6752136752136753</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -3142,16 +3142,16 @@
         <v>198</v>
       </c>
       <c r="D70">
-        <v>0.9989106971538215</v>
+        <v>0.04019760686493977</v>
       </c>
       <c r="E70">
-        <v>0.001089302846178446</v>
+        <v>0.8493797303059375</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>0.1101095299008635</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>0.0003131329282592474</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -3171,13 +3171,13 @@
         <v>199</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>0.7760880964866282</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>0.2233875196643943</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>0.0005243838489774515</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -3200,10 +3200,10 @@
         <v>200</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>0.4102564102564102</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>0.5897435897435898</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -3229,19 +3229,19 @@
         <v>201</v>
       </c>
       <c r="D73">
-        <v>0.9965400939756871</v>
+        <v>0.08209629201308402</v>
       </c>
       <c r="E73">
-        <v>0.003459906024312945</v>
+        <v>0.8186462549620418</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>0.09776354143527428</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>0.001482380830452057</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>1.15307591478769E-05</v>
       </c>
       <c r="I73">
         <v>0</v>
@@ -3258,13 +3258,13 @@
         <v>202</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>0.181110029211295</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>0.7692307692307693</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>0.04965920155793573</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -3287,16 +3287,16 @@
         <v>203</v>
       </c>
       <c r="D75">
-        <v>0.9954892084875701</v>
+        <v>0.1024334000849566</v>
       </c>
       <c r="E75">
-        <v>0.004510791512429961</v>
+        <v>0.4868822946376196</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>0.4101179278677913</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>0.0005663774096324615</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -3316,10 +3316,10 @@
         <v>204</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0.9964774951076321</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>0.003522504892367906</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -3345,13 +3345,13 @@
         <v>205</v>
       </c>
       <c r="D77">
-        <v>0.8571428571428571</v>
+        <v>0</v>
       </c>
       <c r="E77">
-        <v>0.1428571428571428</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -3374,19 +3374,19 @@
         <v>206</v>
       </c>
       <c r="D78">
-        <v>0.9783288450382723</v>
+        <v>0.3059570915848005</v>
       </c>
       <c r="E78">
-        <v>0.02167115496172765</v>
+        <v>0.4722896907556843</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>0.2114906641890649</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>0.0100880523314767</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>0.0001745011389736503</v>
       </c>
       <c r="I78">
         <v>0</v>
@@ -3403,13 +3403,13 @@
         <v>207</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>0.6740975914058234</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>0.3255397666063725</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>0.0003626419878042059</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -3432,22 +3432,22 @@
         <v>208</v>
       </c>
       <c r="D80">
-        <v>0.9628952812509745</v>
+        <v>0.02811335044551036</v>
       </c>
       <c r="E80">
-        <v>0.03710471874902553</v>
+        <v>0.7015163883481709</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>0.2473000051686805</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>0.02258371660594535</v>
       </c>
       <c r="H80">
-        <v>0</v>
+        <v>0.0004861122680127448</v>
       </c>
       <c r="I80">
-        <v>0</v>
+        <v>4.271636801517969E-07</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3461,19 +3461,19 @@
         <v>209</v>
       </c>
       <c r="D81">
-        <v>0.950883562009503</v>
+        <v>0.03288665848059367</v>
       </c>
       <c r="E81">
-        <v>0.04911643799049704</v>
+        <v>0.502482515615824</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>0.4389514708237681</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>0.0253857242005232</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>0.0002936308792910149</v>
       </c>
       <c r="I81">
         <v>0</v>
@@ -3490,13 +3490,13 @@
         <v>210</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>0.4910561062615602</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>0.508802782173816</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>0.000141111564623786</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -3519,16 +3519,16 @@
         <v>211</v>
       </c>
       <c r="D83">
-        <v>0.9977005546110445</v>
+        <v>0.1324153892550466</v>
       </c>
       <c r="E83">
-        <v>0.002299445388955558</v>
+        <v>0.8134165307940417</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>0.05345592398840771</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>0.0007121559625040309</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -3548,13 +3548,13 @@
         <v>212</v>
       </c>
       <c r="D84">
-        <v>0.9999925707174829</v>
+        <v>0.119291989376126</v>
       </c>
       <c r="E84">
-        <v>7.429282517040917E-06</v>
+        <v>0.8626065637711038</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>0.01810144685277019</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -3577,16 +3577,16 @@
         <v>213</v>
       </c>
       <c r="D85">
-        <v>0.9850096711798839</v>
+        <v>0.02659574468085106</v>
       </c>
       <c r="E85">
-        <v>0.01499032882011605</v>
+        <v>0.6576402321083172</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>0.3089941972920696</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>0.006769825918762089</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -3606,19 +3606,19 @@
         <v>214</v>
       </c>
       <c r="D86">
-        <v>0.9937068292556596</v>
+        <v>0.4514027370298158</v>
       </c>
       <c r="E86">
-        <v>0.006293170744340401</v>
+        <v>0.4590536935843695</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>0.08620645003755184</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>0.003307521837413474</v>
       </c>
       <c r="H86">
-        <v>0</v>
+        <v>2.959751084933757E-05</v>
       </c>
       <c r="I86">
         <v>0</v>
@@ -3635,16 +3635,16 @@
         <v>215</v>
       </c>
       <c r="D87">
-        <v>0.9984008195427595</v>
+        <v>0.06513161225383193</v>
       </c>
       <c r="E87">
-        <v>0.001599180457240535</v>
+        <v>0.8277128741471782</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>0.106504822854284</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>0.0006506907447058789</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -3664,10 +3664,10 @@
         <v>216</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>0.03928571428571428</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>0.9607142857142857</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -3693,10 +3693,10 @@
         <v>217</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>0.9999917052373132</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>8.29476268683953E-06</v>
       </c>
       <c r="F89">
         <v>0</v>
@@ -3722,16 +3722,16 @@
         <v>218</v>
       </c>
       <c r="D90">
-        <v>0.9998716302952503</v>
+        <v>0.9980744544287549</v>
       </c>
       <c r="E90">
+        <v>0.001797175866495507</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
         <v>0.0001283697047496791</v>
-      </c>
-      <c r="F90">
-        <v>0</v>
-      </c>
-      <c r="G90">
-        <v>0</v>
       </c>
       <c r="H90">
         <v>0</v>
@@ -3751,22 +3751,22 @@
         <v>219</v>
       </c>
       <c r="D91">
-        <v>0.8241117081399487</v>
+        <v>0.01726723017495107</v>
       </c>
       <c r="E91">
-        <v>0.1758877877073454</v>
+        <v>0.3548025082605421</v>
       </c>
       <c r="F91">
-        <v>5.041527058379875E-07</v>
+        <v>0.5108231502889299</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>0.1098311794249231</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>0.007243666077480205</v>
       </c>
       <c r="I91">
-        <v>0</v>
+        <v>3.22657731736312E-05</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3780,13 +3780,13 @@
         <v>220</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>0.01120269328999303</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>0.9885070814952404</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>0.0002902252147666589</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -3809,19 +3809,19 @@
         <v>221</v>
       </c>
       <c r="D93">
-        <v>0.9952999400580975</v>
+        <v>0.3065567219464211</v>
       </c>
       <c r="E93">
-        <v>0.004700059941902463</v>
+        <v>0.5991454436469268</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>0.09231206676605751</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>0.001942732428569233</v>
       </c>
       <c r="H93">
-        <v>0</v>
+        <v>4.303521202526782E-05</v>
       </c>
       <c r="I93">
         <v>0</v>
@@ -3838,19 +3838,19 @@
         <v>222</v>
       </c>
       <c r="D94">
-        <v>0.9834040296924709</v>
+        <v>0.004697773064687169</v>
       </c>
       <c r="E94">
-        <v>0.01659597030752916</v>
+        <v>0.619704946665835</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>0.3696562909363109</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>0.005884224315388934</v>
       </c>
       <c r="H94">
-        <v>0</v>
+        <v>5.676501777805502E-05</v>
       </c>
       <c r="I94">
         <v>0</v>
@@ -3867,16 +3867,16 @@
         <v>223</v>
       </c>
       <c r="D95">
-        <v>0.9994851770791883</v>
+        <v>0.2997562674094708</v>
       </c>
       <c r="E95">
-        <v>0.0005148229208117788</v>
+        <v>0.6350701352964584</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>0.06509152407481099</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>8.207321925984879E-05</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -3896,19 +3896,19 @@
         <v>224</v>
       </c>
       <c r="D96">
-        <v>0.9602705426437128</v>
+        <v>0.004597354832677063</v>
       </c>
       <c r="E96">
-        <v>0.03972945735628721</v>
+        <v>0.6223363913102201</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>0.3537625583110825</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>0.01914785300931938</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>0.0001558425367009174</v>
       </c>
       <c r="I96">
         <v>0</v>
@@ -3925,13 +3925,13 @@
         <v>225</v>
       </c>
       <c r="D97">
-        <v>0.999979247407223</v>
+        <v>0.9189611252055804</v>
       </c>
       <c r="E97">
-        <v>2.075259277706008E-05</v>
+        <v>0.07853818736478389</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>0.00250068742963574</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -3954,22 +3954,22 @@
         <v>226</v>
       </c>
       <c r="D98">
-        <v>0.8927349727555844</v>
+        <v>0.02359830599377142</v>
       </c>
       <c r="E98">
-        <v>0.1072650272444155</v>
+        <v>0.5831822258544771</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>0.320841114053972</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>0.06919796106309557</v>
       </c>
       <c r="H98">
-        <v>0</v>
+        <v>0.003175886100766028</v>
       </c>
       <c r="I98">
-        <v>0</v>
+        <v>4.506933917832585E-06</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -3983,10 +3983,10 @@
         <v>227</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0.007051282051282051</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>0.992948717948718</v>
       </c>
       <c r="F99">
         <v>0</v>
@@ -4012,13 +4012,13 @@
         <v>228</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>0.2127659574468085</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>0.773936170212766</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>0.01329787234042553</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -4041,10 +4041,10 @@
         <v>229</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="F101">
         <v>0</v>
@@ -4070,13 +4070,13 @@
         <v>230</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>0.664291713922761</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>0.3348230503741427</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>0.0008852357030963086</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -4099,13 +4099,13 @@
         <v>231</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>0.4574257425742574</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>0.5425742574257426</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4128,22 +4128,22 @@
         <v>232</v>
       </c>
       <c r="D104">
-        <v>0.992915242347724</v>
+        <v>0.4603553989352644</v>
       </c>
       <c r="E104">
-        <v>0.007083499545688725</v>
+        <v>0.4600386256695261</v>
       </c>
       <c r="F104">
-        <v>8.087828061402431E-07</v>
+        <v>0.07583183536273415</v>
       </c>
       <c r="G104">
-        <v>4.493237811890239E-07</v>
+        <v>0.003687959731243271</v>
       </c>
       <c r="H104">
-        <v>0</v>
+        <v>8.366408805739626E-05</v>
       </c>
       <c r="I104">
-        <v>0</v>
+        <v>2.516213174658534E-06</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -4157,10 +4157,10 @@
         <v>233</v>
       </c>
       <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
         <v>1</v>
-      </c>
-      <c r="E105">
-        <v>0</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -4186,13 +4186,13 @@
         <v>234</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>0.7861441393217815</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>0.2138532107660631</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>2.649912155412048E-06</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -4215,10 +4215,10 @@
         <v>235</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>0.8781169727576145</v>
       </c>
       <c r="E107">
-        <v>0</v>
+        <v>0.1218830272423856</v>
       </c>
       <c r="F107">
         <v>0</v>
@@ -4244,22 +4244,22 @@
         <v>236</v>
       </c>
       <c r="D108">
-        <v>0.9293523106408285</v>
+        <v>0.02310773277598751</v>
       </c>
       <c r="E108">
-        <v>0.0706476893591715</v>
+        <v>0.5782158311114997</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>0.3557195496200697</v>
       </c>
       <c r="G108">
-        <v>0</v>
+        <v>0.04120855833124726</v>
       </c>
       <c r="H108">
-        <v>0</v>
+        <v>0.00173706998743058</v>
       </c>
       <c r="I108">
-        <v>0</v>
+        <v>1.125817376527635E-05</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -4273,19 +4273,19 @@
         <v>237</v>
       </c>
       <c r="D109">
-        <v>0.8749172404661016</v>
+        <v>0.001655190677966102</v>
       </c>
       <c r="E109">
-        <v>0.1250827595338983</v>
+        <v>0.3359540519067797</v>
       </c>
       <c r="F109">
-        <v>0</v>
+        <v>0.5980369438559322</v>
       </c>
       <c r="G109">
-        <v>0</v>
+        <v>0.06372484110169492</v>
       </c>
       <c r="H109">
-        <v>0</v>
+        <v>0.0006289724576271186</v>
       </c>
       <c r="I109">
         <v>0</v>
@@ -4302,19 +4302,19 @@
         <v>238</v>
       </c>
       <c r="D110">
-        <v>0.990300550982648</v>
+        <v>0.03734544647589678</v>
       </c>
       <c r="E110">
-        <v>0.009699449017351997</v>
+        <v>0.8805551536908197</v>
       </c>
       <c r="F110">
-        <v>0</v>
+        <v>0.07778410323310096</v>
       </c>
       <c r="G110">
-        <v>0</v>
+        <v>0.004296716879926366</v>
       </c>
       <c r="H110">
-        <v>0</v>
+        <v>1.857972025621643E-05</v>
       </c>
       <c r="I110">
         <v>0</v>
@@ -4331,13 +4331,13 @@
         <v>239</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>0.1846153846153846</v>
       </c>
       <c r="E111">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F111">
-        <v>0</v>
+        <v>0.01538461538461539</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -4360,10 +4360,10 @@
         <v>240</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>0.7741935483870968</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>0.2258064516129032</v>
       </c>
       <c r="F112">
         <v>0</v>
@@ -4389,22 +4389,22 @@
         <v>241</v>
       </c>
       <c r="D113">
-        <v>0.9972868870078488</v>
+        <v>0.1844045385093565</v>
       </c>
       <c r="E113">
-        <v>0.002486536104155653</v>
+        <v>0.6645151545080086</v>
       </c>
       <c r="F113">
-        <v>0.0001103836121003678</v>
+        <v>0.1493838851545661</v>
       </c>
       <c r="G113">
-        <v>5.809663794756197E-05</v>
+        <v>0.001039929819261359</v>
       </c>
       <c r="H113">
-        <v>2.904831897378099E-05</v>
+        <v>0.0003427701638906157</v>
       </c>
       <c r="I113">
-        <v>2.904831897378099E-05</v>
+        <v>0.0003137218449168347</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -4418,10 +4418,10 @@
         <v>242</v>
       </c>
       <c r="D114">
-        <v>1</v>
+        <v>0.1409395973154362</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>0.8590604026845637</v>
       </c>
       <c r="F114">
         <v>0</v>
@@ -4447,10 +4447,10 @@
         <v>243</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>0.01076555023923445</v>
       </c>
       <c r="E115">
-        <v>0</v>
+        <v>0.9892344497607656</v>
       </c>
       <c r="F115">
         <v>0</v>
@@ -4476,10 +4476,10 @@
         <v>244</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>0.155688622754491</v>
       </c>
       <c r="E116">
-        <v>0</v>
+        <v>0.844311377245509</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -4505,22 +4505,22 @@
         <v>245</v>
       </c>
       <c r="D117">
-        <v>0.9618877550829487</v>
+        <v>0.0234485654209437</v>
       </c>
       <c r="E117">
-        <v>0.03811224491705138</v>
+        <v>0.6346391539626474</v>
       </c>
       <c r="F117">
-        <v>0</v>
+        <v>0.3228243505542194</v>
       </c>
       <c r="G117">
-        <v>0</v>
+        <v>0.01871072930344716</v>
       </c>
       <c r="H117">
-        <v>0</v>
+        <v>0.0003764523445384661</v>
       </c>
       <c r="I117">
-        <v>0</v>
+        <v>7.484142038538093E-07</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -4534,10 +4534,10 @@
         <v>246</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>0.79346171070309</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>0.20653828929691</v>
       </c>
       <c r="F118">
         <v>0</v>
@@ -4563,10 +4563,10 @@
         <v>247</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>0.06695741405849154</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>0.9330425859415085</v>
       </c>
       <c r="F119">
         <v>0</v>
@@ -4592,19 +4592,19 @@
         <v>248</v>
       </c>
       <c r="D120">
-        <v>0.9224476290447721</v>
+        <v>0.03301994432020446</v>
       </c>
       <c r="E120">
-        <v>0.07755237095522796</v>
+        <v>0.4336634567112409</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>0.495812605540596</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>0.03718451919127379</v>
       </c>
       <c r="H120">
-        <v>0</v>
+        <v>0.0003194742366847702</v>
       </c>
       <c r="I120">
         <v>0</v>
@@ -4621,13 +4621,13 @@
         <v>249</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>0.7539170506912443</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>0.2267281105990784</v>
       </c>
       <c r="F121">
-        <v>0</v>
+        <v>0.01935483870967742</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -4650,13 +4650,13 @@
         <v>250</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>0.4279749478079332</v>
       </c>
       <c r="E122">
-        <v>0</v>
+        <v>0.5121781489213639</v>
       </c>
       <c r="F122">
-        <v>0</v>
+        <v>0.05984690327070286</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -4679,13 +4679,13 @@
         <v>251</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>0.665705871295194</v>
       </c>
       <c r="E123">
-        <v>0</v>
+        <v>0.3161225640704305</v>
       </c>
       <c r="F123">
-        <v>0</v>
+        <v>0.01817156463437559</v>
       </c>
       <c r="G123">
         <v>0</v>

</xml_diff>

<commit_message>
Update to carbon stats.
</commit_message>
<xml_diff>
--- a/07_calc_country_stats/03_total_c_stats/02_combine_tile_stats/country_total_c_hists_summary.xlsx
+++ b/07_calc_country_stats/03_total_c_stats/02_combine_tile_stats/country_total_c_hists_summary.xlsx
@@ -1170,13 +1170,13 @@
         <v>130</v>
       </c>
       <c r="D2">
-        <v>0.02316968853256403</v>
+        <v>0.02365944885191459</v>
       </c>
       <c r="E2">
-        <v>0.7097901746029084</v>
+        <v>0.7105315241274047</v>
       </c>
       <c r="F2">
-        <v>0.2669831099780279</v>
+        <v>0.2657520001341809</v>
       </c>
       <c r="G2">
         <v>5.702688649972325E-05</v>
@@ -1228,13 +1228,13 @@
         <v>132</v>
       </c>
       <c r="D4">
-        <v>0.04010554089709763</v>
+        <v>0.04068015244796248</v>
       </c>
       <c r="E4">
-        <v>0.9334036939313984</v>
+        <v>0.9332277924362357</v>
       </c>
       <c r="F4">
-        <v>0.02649076517150396</v>
+        <v>0.02609205511580182</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1257,10 +1257,10 @@
         <v>133</v>
       </c>
       <c r="D5">
-        <v>0.02305475504322766</v>
+        <v>0.02449567723342939</v>
       </c>
       <c r="E5">
-        <v>0.9740634005763689</v>
+        <v>0.9726224783861671</v>
       </c>
       <c r="F5">
         <v>0.002881844380403458</v>
@@ -1289,13 +1289,13 @@
         <v>5.758948830587851E-07</v>
       </c>
       <c r="E6">
-        <v>0.06152745751623448</v>
+        <v>0.06202791016961256</v>
       </c>
       <c r="F6">
-        <v>0.9364897364013941</v>
+        <v>0.9360290204949471</v>
       </c>
       <c r="G6">
-        <v>0.001982230187488338</v>
+        <v>0.001942493440557282</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1315,13 +1315,13 @@
         <v>135</v>
       </c>
       <c r="D7">
-        <v>0.008901742788461538</v>
+        <v>0.00915214342948718</v>
       </c>
       <c r="E7">
-        <v>0.9118088942307693</v>
+        <v>0.9117462940705128</v>
       </c>
       <c r="F7">
-        <v>0.07811247996794872</v>
+        <v>0.07792467948717949</v>
       </c>
       <c r="G7">
         <v>0.001176883012820513</v>
@@ -1344,13 +1344,13 @@
         <v>136</v>
       </c>
       <c r="D8">
-        <v>6.137570861045395E-05</v>
+        <v>6.509544852623904E-05</v>
       </c>
       <c r="E8">
-        <v>0.5329829338332663</v>
+        <v>0.5357559999404842</v>
       </c>
       <c r="F8">
-        <v>0.4669556904581232</v>
+        <v>0.4641789046109896</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1373,13 +1373,13 @@
         <v>137</v>
       </c>
       <c r="D9">
-        <v>0.009543319936458884</v>
+        <v>0.009796789958420499</v>
       </c>
       <c r="E9">
-        <v>0.9329675957673979</v>
+        <v>0.9333668978567894</v>
       </c>
       <c r="F9">
-        <v>0.05748908429614327</v>
+        <v>0.05683631218479007</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1405,10 +1405,10 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0.07867537451718373</v>
+        <v>0.07980366157976661</v>
       </c>
       <c r="F10">
-        <v>0.9212669757788887</v>
+        <v>0.9201386887163058</v>
       </c>
       <c r="G10">
         <v>5.764970392759197E-05</v>
@@ -1431,13 +1431,13 @@
         <v>139</v>
       </c>
       <c r="D11">
-        <v>0.022823973479332</v>
+        <v>0.02428032574524479</v>
       </c>
       <c r="E11">
-        <v>0.8980761093328556</v>
+        <v>0.8989457671030532</v>
       </c>
       <c r="F11">
-        <v>0.07909991718781233</v>
+        <v>0.07677390715170207</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1460,10 +1460,10 @@
         <v>140</v>
       </c>
       <c r="D12">
-        <v>0.06790518898142217</v>
+        <v>0.06854580397181294</v>
       </c>
       <c r="E12">
-        <v>0.9320948110185778</v>
+        <v>0.931454196028187</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1489,10 +1489,10 @@
         <v>141</v>
       </c>
       <c r="D13">
-        <v>0.3521082981653216</v>
+        <v>0.356532337488135</v>
       </c>
       <c r="E13">
-        <v>0.6478738764432996</v>
+        <v>0.6434498371204863</v>
       </c>
       <c r="F13">
         <v>1.782539137874946E-05</v>
@@ -1518,13 +1518,13 @@
         <v>142</v>
       </c>
       <c r="D14">
-        <v>0.2649618101270709</v>
+        <v>0.2661583260784726</v>
       </c>
       <c r="E14">
-        <v>0.7331940971879731</v>
+        <v>0.7320061584118502</v>
       </c>
       <c r="F14">
-        <v>0.001844092684956064</v>
+        <v>0.001835515509677198</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1547,13 +1547,13 @@
         <v>143</v>
       </c>
       <c r="D15">
-        <v>0.0921746801940891</v>
+        <v>0.09326863696515218</v>
       </c>
       <c r="E15">
-        <v>0.9027613586237319</v>
+        <v>0.9017909131010146</v>
       </c>
       <c r="F15">
-        <v>0.005063961182179091</v>
+        <v>0.004940449933833259</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1576,16 +1576,16 @@
         <v>144</v>
       </c>
       <c r="D16">
-        <v>0.0002565513066580829</v>
+        <v>0.0002656795366702619</v>
       </c>
       <c r="E16">
-        <v>0.6451554321376153</v>
+        <v>0.6461859612626745</v>
       </c>
       <c r="F16">
-        <v>0.3479806193263847</v>
+        <v>0.3469688270945084</v>
       </c>
       <c r="G16">
-        <v>0.006607397229341974</v>
+        <v>0.006579532106146902</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1608,10 +1608,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0.8087788160752356</v>
+        <v>0.8104006854091534</v>
       </c>
       <c r="F17">
-        <v>0.1912211839247644</v>
+        <v>0.1895993145908466</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1663,13 +1663,13 @@
         <v>147</v>
       </c>
       <c r="D19">
-        <v>0.06104548203965923</v>
+        <v>0.06411575656432418</v>
       </c>
       <c r="E19">
-        <v>0.9382498050561511</v>
+        <v>0.9352086810135622</v>
       </c>
       <c r="F19">
-        <v>0.0007047129041896531</v>
+        <v>0.0006755624221135557</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1695,10 +1695,10 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.174096221799402</v>
+        <v>0.1750475672737157</v>
       </c>
       <c r="F20">
-        <v>0.825903778200598</v>
+        <v>0.8249524327262843</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1724,13 +1724,13 @@
         <v>1.429855745428483E-05</v>
       </c>
       <c r="E21">
-        <v>0.1620652121459096</v>
+        <v>0.163879341622922</v>
       </c>
       <c r="F21">
-        <v>0.8348552360423738</v>
+        <v>0.8330536178031339</v>
       </c>
       <c r="G21">
-        <v>0.00306525325426231</v>
+        <v>0.003052742016489811</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1750,13 +1750,13 @@
         <v>150</v>
       </c>
       <c r="D22">
-        <v>0.02178770282218558</v>
+        <v>0.02205653929791861</v>
       </c>
       <c r="E22">
-        <v>0.7029834874662461</v>
+        <v>0.7048533945085669</v>
       </c>
       <c r="F22">
-        <v>0.2752288097115683</v>
+        <v>0.2730900661935144</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1779,16 +1779,16 @@
         <v>151</v>
       </c>
       <c r="D23">
-        <v>0.0002525983067588183</v>
+        <v>0.000261511236543639</v>
       </c>
       <c r="E23">
-        <v>0.1538400084702216</v>
+        <v>0.155097286587487</v>
       </c>
       <c r="F23">
-        <v>0.8376915002547041</v>
+        <v>0.8366010865481721</v>
       </c>
       <c r="G23">
-        <v>0.008215827672126549</v>
+        <v>0.008040050331608328</v>
       </c>
       <c r="H23">
         <v>6.529618889978501E-08</v>
@@ -1808,16 +1808,16 @@
         <v>152</v>
       </c>
       <c r="D24">
-        <v>0.7398347077191147</v>
+        <v>0.74062715910085</v>
       </c>
       <c r="E24">
-        <v>0.1880935016755069</v>
+        <v>0.1876226280017639</v>
       </c>
       <c r="F24">
-        <v>0.07205862399554389</v>
+        <v>0.07173816210194438</v>
       </c>
       <c r="G24">
-        <v>1.316660983452026E-05</v>
+        <v>1.205079544176431E-05</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1837,13 +1837,13 @@
         <v>153</v>
       </c>
       <c r="D25">
-        <v>0.01400116676389699</v>
+        <v>0.01437156800103712</v>
       </c>
       <c r="E25">
-        <v>0.774194145808447</v>
+        <v>0.7752405293033678</v>
       </c>
       <c r="F25">
-        <v>0.211804687427656</v>
+        <v>0.210387902695595</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1869,10 +1869,10 @@
         <v>0.009584664536741214</v>
       </c>
       <c r="E26">
-        <v>0.943248696821927</v>
+        <v>0.9457709769631747</v>
       </c>
       <c r="F26">
-        <v>0.04716663864133176</v>
+        <v>0.04464435850008407</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1895,13 +1895,13 @@
         <v>155</v>
       </c>
       <c r="D27">
-        <v>0.03779277199462727</v>
+        <v>0.03872495522722185</v>
       </c>
       <c r="E27">
-        <v>0.8480891118200135</v>
+        <v>0.847956192634878</v>
       </c>
       <c r="F27">
-        <v>0.1141181161853593</v>
+        <v>0.1133188521379002</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1924,13 +1924,13 @@
         <v>156</v>
       </c>
       <c r="D28">
-        <v>0.008128650468029875</v>
+        <v>0.008315642427375623</v>
       </c>
       <c r="E28">
-        <v>0.8054843641723406</v>
+        <v>0.8066943121445778</v>
       </c>
       <c r="F28">
-        <v>0.1863759858326092</v>
+        <v>0.1849790459010263</v>
       </c>
       <c r="G28">
         <v>1.099952702033813E-05</v>
@@ -1956,10 +1956,10 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0.788692175899486</v>
+        <v>0.7961165048543689</v>
       </c>
       <c r="F29">
-        <v>0.211307824100514</v>
+        <v>0.2038834951456311</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1982,10 +1982,10 @@
         <v>158</v>
       </c>
       <c r="D30">
-        <v>0.1128143581910425</v>
+        <v>0.1141508919317004</v>
       </c>
       <c r="E30">
-        <v>0.8870219846162238</v>
+        <v>0.8856854508755659</v>
       </c>
       <c r="F30">
         <v>0.0001636571927336206</v>
@@ -2011,13 +2011,13 @@
         <v>159</v>
       </c>
       <c r="D31">
-        <v>0.2030198302184344</v>
+        <v>0.2041955851974978</v>
       </c>
       <c r="E31">
-        <v>0.7914374477874797</v>
+        <v>0.7903525458201162</v>
       </c>
       <c r="F31">
-        <v>0.005542721994085951</v>
+        <v>0.005451868982386044</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -2040,13 +2040,13 @@
         <v>160</v>
       </c>
       <c r="D32">
-        <v>0.0009464767403341063</v>
+        <v>0.0009938005773508117</v>
       </c>
       <c r="E32">
-        <v>0.6037575126591264</v>
+        <v>0.6065969428801288</v>
       </c>
       <c r="F32">
-        <v>0.3952960106005395</v>
+        <v>0.3924092565425205</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -2098,16 +2098,16 @@
         <v>162</v>
       </c>
       <c r="D34">
-        <v>5.364465598642645E-05</v>
+        <v>5.581943933722752E-05</v>
       </c>
       <c r="E34">
-        <v>0.2581987973085606</v>
+        <v>0.2614629658861671</v>
       </c>
       <c r="F34">
-        <v>0.7398455287632315</v>
+        <v>0.7366179690386968</v>
       </c>
       <c r="G34">
-        <v>0.001901848040275538</v>
+        <v>0.001863064403852919</v>
       </c>
       <c r="H34">
         <v>1.812319459000894E-07</v>
@@ -2130,10 +2130,10 @@
         <v>0.0009603512141583208</v>
       </c>
       <c r="E35">
-        <v>0.7829606256002195</v>
+        <v>0.7839209768143778</v>
       </c>
       <c r="F35">
-        <v>0.2160790231856222</v>
+        <v>0.2151186719714638</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -2156,13 +2156,13 @@
         <v>164</v>
       </c>
       <c r="D36">
-        <v>0.00014422205731468</v>
+        <v>0.0001526791756091296</v>
       </c>
       <c r="E36">
-        <v>0.785139692988564</v>
+        <v>0.7864411871132913</v>
       </c>
       <c r="F36">
-        <v>0.2147152956230804</v>
+        <v>0.2134053443800588</v>
       </c>
       <c r="G36">
         <v>7.893310408152933E-07</v>
@@ -2185,13 +2185,13 @@
         <v>165</v>
       </c>
       <c r="D37">
-        <v>0.02269138691880427</v>
+        <v>0.0231213368576766</v>
       </c>
       <c r="E37">
-        <v>0.8924826057209513</v>
+        <v>0.8929175405866511</v>
       </c>
       <c r="F37">
-        <v>0.08482600736024445</v>
+        <v>0.08396112255567229</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2243,13 +2243,13 @@
         <v>167</v>
       </c>
       <c r="D39">
-        <v>0.117883307291423</v>
+        <v>0.1192458293958589</v>
       </c>
       <c r="E39">
-        <v>0.8618578018132654</v>
+        <v>0.86075725820788</v>
       </c>
       <c r="F39">
-        <v>0.02025421270782848</v>
+        <v>0.01999223420877815</v>
       </c>
       <c r="G39">
         <v>4.678187483041571E-06</v>
@@ -2301,13 +2301,13 @@
         <v>169</v>
       </c>
       <c r="D41">
-        <v>0.02753840389659048</v>
+        <v>0.02772573997751967</v>
       </c>
       <c r="E41">
-        <v>0.9514799550393406</v>
+        <v>0.9520419632821281</v>
       </c>
       <c r="F41">
-        <v>0.02098164106406894</v>
+        <v>0.02023229674035219</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2330,13 +2330,13 @@
         <v>170</v>
       </c>
       <c r="D42">
-        <v>0.117958364685227</v>
+        <v>0.1187358916478555</v>
       </c>
       <c r="E42">
-        <v>0.8730248306997742</v>
+        <v>0.8723100075244544</v>
       </c>
       <c r="F42">
-        <v>0.009016804614998746</v>
+        <v>0.008954100827689992</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -2388,10 +2388,10 @@
         <v>172</v>
       </c>
       <c r="D44">
-        <v>0.07352128247650636</v>
+        <v>0.07462686567164178</v>
       </c>
       <c r="E44">
-        <v>0.9264787175234936</v>
+        <v>0.9253731343283582</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -2417,13 +2417,13 @@
         <v>173</v>
       </c>
       <c r="D45">
-        <v>0.03088086167676159</v>
+        <v>0.03122773179488585</v>
       </c>
       <c r="E45">
-        <v>0.9010186847370296</v>
+        <v>0.9011762751116836</v>
       </c>
       <c r="F45">
-        <v>0.06809959711678132</v>
+        <v>0.06759513662400307</v>
       </c>
       <c r="G45">
         <v>8.564694274673171E-07</v>
@@ -2446,16 +2446,16 @@
         <v>174</v>
       </c>
       <c r="D46">
-        <v>0.0004477532567169497</v>
+        <v>0.0004566785708043307</v>
       </c>
       <c r="E46">
-        <v>0.2413323113848703</v>
+        <v>0.2430634504297353</v>
       </c>
       <c r="F46">
-        <v>0.7581723336832801</v>
+        <v>0.7564330131005016</v>
       </c>
       <c r="G46">
-        <v>4.760167513269897E-05</v>
+        <v>4.685789895875055E-05</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -2504,13 +2504,13 @@
         <v>176</v>
       </c>
       <c r="D48">
-        <v>0.01377331250435948</v>
+        <v>0.01394242727735744</v>
       </c>
       <c r="E48">
-        <v>0.8562639585491137</v>
+        <v>0.8571868514251045</v>
       </c>
       <c r="F48">
-        <v>0.1299627289465268</v>
+        <v>0.128870721297538</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2533,10 +2533,10 @@
         <v>177</v>
       </c>
       <c r="D49">
-        <v>0.1250476069569633</v>
+        <v>0.1262536498667005</v>
       </c>
       <c r="E49">
-        <v>0.8747619652151835</v>
+        <v>0.8735559223054462</v>
       </c>
       <c r="F49">
         <v>0.0001904278278532436</v>
@@ -2565,10 +2565,10 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>0.7489451476793249</v>
+        <v>0.7531645569620253</v>
       </c>
       <c r="F50">
-        <v>0.2510548523206751</v>
+        <v>0.2468354430379747</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2591,13 +2591,13 @@
         <v>179</v>
       </c>
       <c r="D51">
-        <v>0.01225369238831257</v>
+        <v>0.01246483136863848</v>
       </c>
       <c r="E51">
-        <v>0.9343027071578658</v>
+        <v>0.9351701576673976</v>
       </c>
       <c r="F51">
-        <v>0.05344360045382161</v>
+        <v>0.05236501096396392</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -2620,13 +2620,13 @@
         <v>180</v>
       </c>
       <c r="D52">
-        <v>0.004183642976363146</v>
+        <v>0.004258036723870265</v>
       </c>
       <c r="E52">
-        <v>0.6146984451958101</v>
+        <v>0.6180044430157717</v>
       </c>
       <c r="F52">
-        <v>0.3811088639396164</v>
+        <v>0.3777284723721477</v>
       </c>
       <c r="G52">
         <v>9.047888210325198E-06</v>
@@ -2736,13 +2736,13 @@
         <v>184</v>
       </c>
       <c r="D56">
-        <v>0.001651240736754712</v>
+        <v>0.001681375111466437</v>
       </c>
       <c r="E56">
-        <v>0.6539374557977922</v>
+        <v>0.6557449032932566</v>
       </c>
       <c r="F56">
-        <v>0.3444026936441069</v>
+        <v>0.3425651117739307</v>
       </c>
       <c r="G56">
         <v>8.609821346207066E-06</v>
@@ -2765,13 +2765,13 @@
         <v>185</v>
       </c>
       <c r="D57">
-        <v>0.004074383618888425</v>
+        <v>0.004178854993731718</v>
       </c>
       <c r="E57">
-        <v>0.7884454659423318</v>
+        <v>0.7915796071876305</v>
       </c>
       <c r="F57">
-        <v>0.2074801504387798</v>
+        <v>0.2042415378186377</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -2794,16 +2794,16 @@
         <v>186</v>
       </c>
       <c r="D58">
-        <v>0.04953236578803451</v>
+        <v>0.05076020963390886</v>
       </c>
       <c r="E58">
-        <v>0.8722311346739243</v>
+        <v>0.8715375849849754</v>
       </c>
       <c r="F58">
-        <v>0.07814835640228528</v>
+        <v>0.07761804816311245</v>
       </c>
       <c r="G58">
-        <v>8.814313575591978E-05</v>
+        <v>8.415721800333965E-05</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -2881,10 +2881,10 @@
         <v>189</v>
       </c>
       <c r="D61">
-        <v>0.7659314835803782</v>
+        <v>0.7672107151216803</v>
       </c>
       <c r="E61">
-        <v>0.2340655684286678</v>
+        <v>0.2327863368873657</v>
       </c>
       <c r="F61">
         <v>2.947990953991491E-06</v>
@@ -2910,10 +2910,10 @@
         <v>190</v>
       </c>
       <c r="D62">
-        <v>0.2099447513812155</v>
+        <v>0.2103697407564811</v>
       </c>
       <c r="E62">
-        <v>0.7896302592435189</v>
+        <v>0.7892052698682533</v>
       </c>
       <c r="F62">
         <v>0.0004249893752656184</v>
@@ -2942,10 +2942,10 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>0.4853547877120984</v>
+        <v>0.4855605245205791</v>
       </c>
       <c r="F63">
-        <v>0.5143420212017196</v>
+        <v>0.5141362843932389</v>
       </c>
       <c r="G63">
         <v>0.0003031910861820662</v>
@@ -2968,16 +2968,16 @@
         <v>192</v>
       </c>
       <c r="D64">
-        <v>1.852804492069997E-05</v>
+        <v>1.961792991603526E-05</v>
       </c>
       <c r="E64">
-        <v>0.4724733196153142</v>
+        <v>0.4746558143184731</v>
       </c>
       <c r="F64">
-        <v>0.454398121910176</v>
+        <v>0.4526259689077609</v>
       </c>
       <c r="G64">
-        <v>0.07311003042958907</v>
+        <v>0.07269859884384999</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -2997,13 +2997,13 @@
         <v>193</v>
       </c>
       <c r="D65">
-        <v>0.3481734492778259</v>
+        <v>0.3514987968191404</v>
       </c>
       <c r="E65">
-        <v>0.6055372879825339</v>
+        <v>0.6023234936334999</v>
       </c>
       <c r="F65">
-        <v>0.04628926273964016</v>
+        <v>0.04617770954735964</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -3026,13 +3026,13 @@
         <v>194</v>
       </c>
       <c r="D66">
-        <v>0.5156398104265403</v>
+        <v>0.5172015924170617</v>
       </c>
       <c r="E66">
-        <v>0.4815520758293839</v>
+        <v>0.4800585402843602</v>
       </c>
       <c r="F66">
-        <v>0.002808113744075829</v>
+        <v>0.002739867298578199</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -3084,13 +3084,13 @@
         <v>196</v>
       </c>
       <c r="D68">
-        <v>0.06643353694563685</v>
+        <v>0.06739140608244008</v>
       </c>
       <c r="E68">
-        <v>0.8723201368152972</v>
+        <v>0.8722871467604345</v>
       </c>
       <c r="F68">
-        <v>0.06124607819354067</v>
+        <v>0.06032119911160014</v>
       </c>
       <c r="G68">
         <v>2.480455252835284E-07</v>
@@ -3142,13 +3142,13 @@
         <v>198</v>
       </c>
       <c r="D70">
-        <v>0.03863860462637245</v>
+        <v>0.03904501119283658</v>
       </c>
       <c r="E70">
-        <v>0.8317643374906727</v>
+        <v>0.8338629943502824</v>
       </c>
       <c r="F70">
-        <v>0.1295970578829549</v>
+        <v>0.1270919944568809</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -3171,10 +3171,10 @@
         <v>199</v>
       </c>
       <c r="D71">
-        <v>0.01651809124278972</v>
+        <v>0.01704247509176718</v>
       </c>
       <c r="E71">
-        <v>0.9834819087572103</v>
+        <v>0.9829575249082328</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -3229,16 +3229,16 @@
         <v>201</v>
       </c>
       <c r="D73">
-        <v>0.0001217512510025825</v>
+        <v>0.0001248035107770206</v>
       </c>
       <c r="E73">
-        <v>0.5015866663727454</v>
+        <v>0.5033559596219945</v>
       </c>
       <c r="F73">
-        <v>0.4979025888249987</v>
+        <v>0.4961336347157244</v>
       </c>
       <c r="G73">
-        <v>0.0003889935512533766</v>
+        <v>0.000385602151504001</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -3261,10 +3261,10 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>0.3398247322297955</v>
+        <v>0.3407984420642649</v>
       </c>
       <c r="F74">
-        <v>0.6514118792599806</v>
+        <v>0.6504381694255112</v>
       </c>
       <c r="G74">
         <v>0.008763388510223954</v>
@@ -3290,10 +3290,10 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>0.1095738009992516</v>
+        <v>0.1100997228796246</v>
       </c>
       <c r="F75">
-        <v>0.8904261990007484</v>
+        <v>0.8899002771203754</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -3316,10 +3316,10 @@
         <v>204</v>
       </c>
       <c r="D76">
-        <v>0.02935420743639922</v>
+        <v>0.03026744944553164</v>
       </c>
       <c r="E76">
-        <v>0.9698630136986301</v>
+        <v>0.9689497716894977</v>
       </c>
       <c r="F76">
         <v>0.0007827788649706458</v>
@@ -3374,13 +3374,13 @@
         <v>206</v>
       </c>
       <c r="D78">
-        <v>0.0233218414114784</v>
+        <v>0.02351992378544849</v>
       </c>
       <c r="E78">
-        <v>0.7208830700881467</v>
+        <v>0.7219819556389807</v>
       </c>
       <c r="F78">
-        <v>0.255795088500375</v>
+        <v>0.2544981205755708</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -3403,16 +3403,16 @@
         <v>207</v>
       </c>
       <c r="D79">
-        <v>0.01051223337358513</v>
+        <v>0.01072142581559999</v>
       </c>
       <c r="E79">
-        <v>0.858043512027939</v>
+        <v>0.8592122338746448</v>
       </c>
       <c r="F79">
-        <v>0.1313597007671225</v>
+        <v>0.1299836654524319</v>
       </c>
       <c r="G79">
-        <v>8.455383135331226E-05</v>
+        <v>8.267485732323865E-05</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -3432,13 +3432,13 @@
         <v>208</v>
       </c>
       <c r="D80">
-        <v>0.2992563507492237</v>
+        <v>0.3033703641527657</v>
       </c>
       <c r="E80">
-        <v>0.6999093985834398</v>
+        <v>0.6957996568166994</v>
       </c>
       <c r="F80">
-        <v>0.0008342506673364593</v>
+        <v>0.0008299790305349413</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -3464,10 +3464,10 @@
         <v>0</v>
       </c>
       <c r="E81">
-        <v>0.4010997811115263</v>
+        <v>0.4040360899044365</v>
       </c>
       <c r="F81">
-        <v>0.5989002188884737</v>
+        <v>0.5959639100955635</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -3490,13 +3490,13 @@
         <v>210</v>
       </c>
       <c r="D82">
-        <v>0.4415684322808636</v>
+        <v>0.4455696279358413</v>
       </c>
       <c r="E82">
-        <v>0.5583056294410313</v>
+        <v>0.5543120204293129</v>
       </c>
       <c r="F82">
-        <v>0.0001259382781050993</v>
+        <v>0.000118351634845756</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -3519,13 +3519,13 @@
         <v>211</v>
       </c>
       <c r="D83">
-        <v>0.08282423196008584</v>
+        <v>0.08410611224618787</v>
       </c>
       <c r="E83">
-        <v>0.8985831061341855</v>
+        <v>0.8973245580890964</v>
       </c>
       <c r="F83">
-        <v>0.01859266190572869</v>
+        <v>0.0185693296647157</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -3548,16 +3548,16 @@
         <v>212</v>
       </c>
       <c r="D84">
-        <v>0.0003863226908861277</v>
+        <v>0.00040489589717873</v>
       </c>
       <c r="E84">
-        <v>0.7311491242733233</v>
+        <v>0.7322709459333965</v>
       </c>
       <c r="F84">
-        <v>0.2632417674263108</v>
+        <v>0.2621050872012036</v>
       </c>
       <c r="G84">
-        <v>0.005222785609479764</v>
+        <v>0.005219070968221244</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -3580,10 +3580,10 @@
         <v>0.002417794970986461</v>
       </c>
       <c r="E85">
-        <v>0.9666344294003868</v>
+        <v>0.9676015473887815</v>
       </c>
       <c r="F85">
-        <v>0.03094777562862669</v>
+        <v>0.02998065764023211</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -3606,13 +3606,13 @@
         <v>214</v>
       </c>
       <c r="D86">
-        <v>0.2428068799413969</v>
+        <v>0.2451524826762069</v>
       </c>
       <c r="E86">
-        <v>0.672818016004854</v>
+        <v>0.6711642550861473</v>
       </c>
       <c r="F86">
-        <v>0.08437510405374908</v>
+        <v>0.08368326223764581</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -3635,13 +3635,13 @@
         <v>215</v>
       </c>
       <c r="D87">
-        <v>0.1919939725488911</v>
+        <v>0.1935857080319359</v>
       </c>
       <c r="E87">
-        <v>0.8020500480945333</v>
+        <v>0.8005268063740891</v>
       </c>
       <c r="F87">
-        <v>0.00595597935657555</v>
+        <v>0.005887485593974931</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -3693,13 +3693,13 @@
         <v>217</v>
       </c>
       <c r="D89">
-        <v>0.01660611489905274</v>
+        <v>0.0169544949319</v>
       </c>
       <c r="E89">
-        <v>0.9749747009738051</v>
+        <v>0.9748171004827552</v>
       </c>
       <c r="F89">
-        <v>0.008419184127142123</v>
+        <v>0.008228404585344812</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -3722,10 +3722,10 @@
         <v>218</v>
       </c>
       <c r="D90">
-        <v>0.02798459563543004</v>
+        <v>0.02875481386392811</v>
       </c>
       <c r="E90">
-        <v>0.9707317073170731</v>
+        <v>0.969961489088575</v>
       </c>
       <c r="F90">
         <v>0.001283697047496791</v>
@@ -3751,13 +3751,13 @@
         <v>219</v>
       </c>
       <c r="D91">
-        <v>0.2058561370004729</v>
+        <v>0.2082357377720282</v>
       </c>
       <c r="E91">
-        <v>0.7930463225589178</v>
+        <v>0.7906783172995968</v>
       </c>
       <c r="F91">
-        <v>0.001097540440609299</v>
+        <v>0.001085944928375025</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -3783,10 +3783,10 @@
         <v>0</v>
       </c>
       <c r="E92">
-        <v>0.7086719294172278</v>
+        <v>0.7122707220803344</v>
       </c>
       <c r="F92">
-        <v>0.2913280705827722</v>
+        <v>0.2877292779196657</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -3809,13 +3809,13 @@
         <v>221</v>
       </c>
       <c r="D93">
-        <v>0.0407774003657993</v>
+        <v>0.04131534051611515</v>
       </c>
       <c r="E93">
-        <v>0.8160121728171157</v>
+        <v>0.8168882467762015</v>
       </c>
       <c r="F93">
-        <v>0.143210426817085</v>
+        <v>0.1417964127076833</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -3838,13 +3838,13 @@
         <v>222</v>
       </c>
       <c r="D94">
-        <v>0.08727964568648244</v>
+        <v>0.08959640696151207</v>
       </c>
       <c r="E94">
-        <v>0.9107073794523112</v>
+        <v>0.9084423928638263</v>
       </c>
       <c r="F94">
-        <v>0.002012974861206412</v>
+        <v>0.001961200174661593</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -3867,13 +3867,13 @@
         <v>223</v>
       </c>
       <c r="D95">
-        <v>0.1928148627138878</v>
+        <v>0.194200159172304</v>
       </c>
       <c r="E95">
-        <v>0.8000049741345006</v>
+        <v>0.7986569836848388</v>
       </c>
       <c r="F95">
-        <v>0.00718016315161162</v>
+        <v>0.007142857142857143</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -3896,13 +3896,13 @@
         <v>224</v>
       </c>
       <c r="D96">
-        <v>0.09119905247737686</v>
+        <v>0.09473148330926431</v>
       </c>
       <c r="E96">
-        <v>0.9084580939418812</v>
+        <v>0.9049308578612171</v>
       </c>
       <c r="F96">
-        <v>0.0003428535807420183</v>
+        <v>0.0003376588295186544</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -3925,13 +3925,13 @@
         <v>225</v>
       </c>
       <c r="D97">
-        <v>0.0207058994433117</v>
+        <v>0.02127659574468085</v>
       </c>
       <c r="E97">
-        <v>0.9444868143213643</v>
+        <v>0.9445490720996954</v>
       </c>
       <c r="F97">
-        <v>0.03480728623532402</v>
+        <v>0.0341743321556237</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -3954,13 +3954,13 @@
         <v>226</v>
       </c>
       <c r="D98">
-        <v>0.03095662677028609</v>
+        <v>0.0321028902967215</v>
       </c>
       <c r="E98">
-        <v>0.9669296212222505</v>
+        <v>0.965838943214135</v>
       </c>
       <c r="F98">
-        <v>0.002113752007463483</v>
+        <v>0.002058166489143547</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -4070,13 +4070,13 @@
         <v>230</v>
       </c>
       <c r="D102">
-        <v>0.1782616126032706</v>
+        <v>0.1798575491135578</v>
       </c>
       <c r="E102">
-        <v>0.8130956044642589</v>
+        <v>0.8115594990451818</v>
       </c>
       <c r="F102">
-        <v>0.008642452373955559</v>
+        <v>0.008582621282745539</v>
       </c>
       <c r="G102">
         <v>3.305585149724827E-07</v>
@@ -4128,16 +4128,16 @@
         <v>232</v>
       </c>
       <c r="D104">
-        <v>0.1997939760598492</v>
+        <v>0.2014602483700106</v>
       </c>
       <c r="E104">
-        <v>0.7299100372911779</v>
+        <v>0.7286126598053727</v>
       </c>
       <c r="F104">
-        <v>0.07029293124726081</v>
+        <v>0.06992421615241709</v>
       </c>
       <c r="G104">
-        <v>3.055401712085363E-06</v>
+        <v>2.875672199609754E-06</v>
       </c>
       <c r="H104">
         <v>0</v>
@@ -4186,13 +4186,13 @@
         <v>234</v>
       </c>
       <c r="D106">
-        <v>0.005572765262831537</v>
+        <v>0.005681411661203431</v>
       </c>
       <c r="E106">
-        <v>0.9621354052113172</v>
+        <v>0.9624242456362572</v>
       </c>
       <c r="F106">
-        <v>0.03229182952585122</v>
+        <v>0.03189434270253941</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -4215,10 +4215,10 @@
         <v>235</v>
       </c>
       <c r="D107">
-        <v>0.00304052283013263</v>
+        <v>0.003180316983242176</v>
       </c>
       <c r="E107">
-        <v>0.9967148374019257</v>
+        <v>0.9965750432488161</v>
       </c>
       <c r="F107">
         <v>0.0002446397679417058</v>
@@ -4244,16 +4244,16 @@
         <v>236</v>
       </c>
       <c r="D108">
-        <v>0.002482427315243435</v>
+        <v>0.002559247795053556</v>
       </c>
       <c r="E108">
-        <v>0.5654798564781519</v>
+        <v>0.5683682402944609</v>
       </c>
       <c r="F108">
-        <v>0.4320191733321678</v>
+        <v>0.4290572802636267</v>
       </c>
       <c r="G108">
-        <v>1.854287443692575E-05</v>
+        <v>1.523164685890329E-05</v>
       </c>
       <c r="H108">
         <v>0</v>
@@ -4276,13 +4276,13 @@
         <v>0</v>
       </c>
       <c r="E109">
-        <v>0.002515889830508474</v>
+        <v>0.002697960805084746</v>
       </c>
       <c r="F109">
-        <v>0.8655157574152542</v>
+        <v>0.8656481726694916</v>
       </c>
       <c r="G109">
-        <v>0.1319518008474576</v>
+        <v>0.1316373146186441</v>
       </c>
       <c r="H109">
         <v>1.655190677966102E-05</v>
@@ -4302,16 +4302,16 @@
         <v>238</v>
       </c>
       <c r="D110">
-        <v>0.0001448800658181371</v>
+        <v>0.000153439262790102</v>
       </c>
       <c r="E110">
-        <v>0.3098562910828407</v>
+        <v>0.3114180313888716</v>
       </c>
       <c r="F110">
-        <v>0.682820794005389</v>
+        <v>0.6812820173985511</v>
       </c>
       <c r="G110">
-        <v>0.0071780348459522</v>
+        <v>0.007146511949787158</v>
       </c>
       <c r="H110">
         <v>0</v>
@@ -4392,13 +4392,13 @@
         <v>0</v>
       </c>
       <c r="E113">
-        <v>0.03557133147043275</v>
+        <v>0.03618132490574149</v>
       </c>
       <c r="F113">
-        <v>0.9631970627363725</v>
+        <v>0.9626103071462183</v>
       </c>
       <c r="G113">
-        <v>0.001231605793194797</v>
+        <v>0.001208367948040178</v>
       </c>
       <c r="H113">
         <v>0</v>
@@ -4505,13 +4505,13 @@
         <v>245</v>
       </c>
       <c r="D117">
-        <v>0.01578068769535949</v>
+        <v>0.01645987358535683</v>
       </c>
       <c r="E117">
-        <v>0.9795177742760309</v>
+        <v>0.9789115587709093</v>
       </c>
       <c r="F117">
-        <v>0.00470153802860963</v>
+        <v>0.004628567643733883</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -4534,13 +4534,13 @@
         <v>246</v>
       </c>
       <c r="D118">
-        <v>0.006090461262875056</v>
+        <v>0.006180026869682042</v>
       </c>
       <c r="E118">
-        <v>0.8744290192566054</v>
+        <v>0.8746081504702194</v>
       </c>
       <c r="F118">
-        <v>0.1194805194805195</v>
+        <v>0.1192118226600985</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -4595,10 +4595,10 @@
         <v>0.0007644562092099859</v>
       </c>
       <c r="E120">
-        <v>0.9643443932271462</v>
+        <v>0.9649262927296791</v>
       </c>
       <c r="F120">
-        <v>0.03489115056364383</v>
+        <v>0.03430925106111086</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -4650,13 +4650,13 @@
         <v>250</v>
       </c>
       <c r="D122">
-        <v>0.003479471120389701</v>
+        <v>0.003827418232428671</v>
       </c>
       <c r="E122">
-        <v>0.8990953375086986</v>
+        <v>0.9008350730688935</v>
       </c>
       <c r="F122">
-        <v>0.09742519137091162</v>
+        <v>0.0953375086986778</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -4679,13 +4679,13 @@
         <v>251</v>
       </c>
       <c r="D123">
-        <v>0.1485055454602419</v>
+        <v>0.1511686195876935</v>
       </c>
       <c r="E123">
-        <v>0.7539946111911774</v>
+        <v>0.7516448399022495</v>
       </c>
       <c r="F123">
-        <v>0.097437182780876</v>
+        <v>0.09712387994235228</v>
       </c>
       <c r="G123">
         <v>6.26605677047434E-05</v>

</xml_diff>